<commit_message>
configurando el analisis de categorías CD
</commit_message>
<xml_diff>
--- a/data/output/Comparacion_categoria_C_y_D/Comparacion_Categorias_C_y_D_25022026.xlsx
+++ b/data/output/Comparacion_categoria_C_y_D/Comparacion_Categorias_C_y_D_25022026.xlsx
@@ -505,7 +505,7 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Fecha de comparación: 25/02/2026 03:00</t>
+          <t>Fecha de comparación: 25/02/2026 19:16</t>
         </is>
       </c>
     </row>
@@ -552,22 +552,22 @@
       <c r="A6" s="5" t="inlineStr"/>
       <c r="B6" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C6" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D6" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E6" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F6" s="6" t="inlineStr">
@@ -580,22 +580,22 @@
       <c r="A7" s="5" t="inlineStr"/>
       <c r="B7" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C7" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D7" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E7" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F7" s="6" t="inlineStr">
@@ -608,22 +608,22 @@
       <c r="A8" s="5" t="inlineStr"/>
       <c r="B8" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C8" s="5" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D8" s="5" t="inlineStr">
         <is>
-          <t>77</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E8" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F8" s="6" t="inlineStr">
@@ -636,7 +636,7 @@
       <c r="A9" s="5" t="inlineStr"/>
       <c r="B9" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C9" s="5" t="inlineStr">
@@ -664,17 +664,17 @@
       <c r="A10" s="5" t="inlineStr"/>
       <c r="B10" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C10" s="5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>77</t>
         </is>
       </c>
       <c r="D10" s="5" t="inlineStr">
         <is>
-          <t>5</t>
+          <t>77</t>
         </is>
       </c>
       <c r="E10" s="5" t="inlineStr">
@@ -692,17 +692,17 @@
       <c r="A11" s="5" t="inlineStr"/>
       <c r="B11" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C11" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="D11" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>5</t>
         </is>
       </c>
       <c r="E11" s="5" t="inlineStr">
@@ -719,7 +719,7 @@
     <row r="13">
       <c r="A13" s="4" t="inlineStr">
         <is>
-          <t>DECO_INTERIOR</t>
+          <t>SEMILLAS</t>
         </is>
       </c>
     </row>
@@ -727,22 +727,22 @@
       <c r="A14" s="5" t="inlineStr"/>
       <c r="B14" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C14" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D14" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E14" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F14" s="6" t="inlineStr">
@@ -755,22 +755,22 @@
       <c r="A15" s="5" t="inlineStr"/>
       <c r="B15" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C15" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D15" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E15" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F15" s="6" t="inlineStr">
@@ -783,27 +783,27 @@
       <c r="A16" s="5" t="inlineStr"/>
       <c r="B16" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C16" s="5" t="inlineStr">
         <is>
-          <t>717</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D16" s="5" t="inlineStr">
         <is>
-          <t>718</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E16" s="5" t="inlineStr">
         <is>
-          <t>+1</t>
-        </is>
-      </c>
-      <c r="F16" s="7" t="inlineStr">
-        <is>
-          <t>↑</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F16" s="6" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -811,17 +811,17 @@
       <c r="A17" s="5" t="inlineStr"/>
       <c r="B17" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C17" s="5" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D17" s="5" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>23</t>
         </is>
       </c>
       <c r="E17" s="5" t="inlineStr">
@@ -839,17 +839,17 @@
       <c r="A18" s="5" t="inlineStr"/>
       <c r="B18" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C18" s="5" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>230</t>
         </is>
       </c>
       <c r="D18" s="5" t="inlineStr">
         <is>
-          <t>110</t>
+          <t>230</t>
         </is>
       </c>
       <c r="E18" s="5" t="inlineStr">
@@ -867,17 +867,17 @@
       <c r="A19" s="5" t="inlineStr"/>
       <c r="B19" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C19" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>23</t>
         </is>
       </c>
       <c r="D19" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>23</t>
         </is>
       </c>
       <c r="E19" s="5" t="inlineStr">
@@ -894,7 +894,7 @@
     <row r="21">
       <c r="A21" s="4" t="inlineStr">
         <is>
-          <t>SEMILLAS</t>
+          <t>DECO_INTERIOR</t>
         </is>
       </c>
     </row>
@@ -902,22 +902,22 @@
       <c r="A22" s="5" t="inlineStr"/>
       <c r="B22" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C22" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D22" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E22" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F22" s="6" t="inlineStr">
@@ -930,22 +930,22 @@
       <c r="A23" s="5" t="inlineStr"/>
       <c r="B23" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C23" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D23" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E23" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F23" s="6" t="inlineStr">
@@ -958,22 +958,22 @@
       <c r="A24" s="5" t="inlineStr"/>
       <c r="B24" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C24" s="5" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D24" s="5" t="inlineStr">
         <is>
-          <t>230</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E24" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F24" s="6" t="inlineStr">
@@ -986,17 +986,17 @@
       <c r="A25" s="5" t="inlineStr"/>
       <c r="B25" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C25" s="5" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>110</t>
         </is>
       </c>
       <c r="D25" s="5" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>110</t>
         </is>
       </c>
       <c r="E25" s="5" t="inlineStr">
@@ -1014,27 +1014,27 @@
       <c r="A26" s="5" t="inlineStr"/>
       <c r="B26" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C26" s="5" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>717</t>
         </is>
       </c>
       <c r="D26" s="5" t="inlineStr">
         <is>
-          <t>23</t>
+          <t>718</t>
         </is>
       </c>
       <c r="E26" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
-        </is>
-      </c>
-      <c r="F26" s="6" t="inlineStr">
-        <is>
-          <t>=</t>
+          <t>+1</t>
+        </is>
+      </c>
+      <c r="F26" s="7" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
     </row>
@@ -1042,17 +1042,17 @@
       <c r="A27" s="5" t="inlineStr"/>
       <c r="B27" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C27" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>110</t>
         </is>
       </c>
       <c r="D27" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>110</t>
         </is>
       </c>
       <c r="E27" s="5" t="inlineStr">
@@ -1069,7 +1069,7 @@
     <row r="29">
       <c r="A29" s="4" t="inlineStr">
         <is>
-          <t>TIERRA_ARIDOS</t>
+          <t>DECO_EXTERIOR</t>
         </is>
       </c>
     </row>
@@ -1077,22 +1077,22 @@
       <c r="A30" s="5" t="inlineStr"/>
       <c r="B30" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C30" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D30" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E30" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F30" s="6" t="inlineStr">
@@ -1105,22 +1105,22 @@
       <c r="A31" s="5" t="inlineStr"/>
       <c r="B31" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C31" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D31" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E31" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F31" s="6" t="inlineStr">
@@ -1133,22 +1133,22 @@
       <c r="A32" s="5" t="inlineStr"/>
       <c r="B32" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C32" s="5" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D32" s="5" t="inlineStr">
         <is>
-          <t>1998</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E32" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F32" s="6" t="inlineStr">
@@ -1161,27 +1161,27 @@
       <c r="A33" s="5" t="inlineStr"/>
       <c r="B33" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C33" s="5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>52</t>
         </is>
       </c>
       <c r="D33" s="5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E33" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
-        </is>
-      </c>
-      <c r="F33" s="6" t="inlineStr">
-        <is>
-          <t>=</t>
+          <t>+10</t>
+        </is>
+      </c>
+      <c r="F33" s="7" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
     </row>
@@ -1189,27 +1189,27 @@
       <c r="A34" s="5" t="inlineStr"/>
       <c r="B34" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C34" s="5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>1753</t>
         </is>
       </c>
       <c r="D34" s="5" t="inlineStr">
         <is>
-          <t>22</t>
+          <t>1542</t>
         </is>
       </c>
       <c r="E34" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
-        </is>
-      </c>
-      <c r="F34" s="6" t="inlineStr">
-        <is>
-          <t>=</t>
+          <t>-211</t>
+        </is>
+      </c>
+      <c r="F34" s="8" t="inlineStr">
+        <is>
+          <t>↓</t>
         </is>
       </c>
     </row>
@@ -1217,34 +1217,34 @@
       <c r="A35" s="5" t="inlineStr"/>
       <c r="B35" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C35" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>52</t>
         </is>
       </c>
       <c r="D35" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>62</t>
         </is>
       </c>
       <c r="E35" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
-        </is>
-      </c>
-      <c r="F35" s="6" t="inlineStr">
-        <is>
-          <t>=</t>
+          <t>+10</t>
+        </is>
+      </c>
+      <c r="F35" s="7" t="inlineStr">
+        <is>
+          <t>↑</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" s="4" t="inlineStr">
         <is>
-          <t>MASCOTAS_VIVO</t>
+          <t>MASCOTAS_MANUFACTURADO</t>
         </is>
       </c>
     </row>
@@ -1252,22 +1252,22 @@
       <c r="A38" s="5" t="inlineStr"/>
       <c r="B38" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C38" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D38" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E38" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F38" s="6" t="inlineStr">
@@ -1280,22 +1280,22 @@
       <c r="A39" s="5" t="inlineStr"/>
       <c r="B39" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C39" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D39" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E39" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F39" s="6" t="inlineStr">
@@ -1308,22 +1308,22 @@
       <c r="A40" s="5" t="inlineStr"/>
       <c r="B40" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C40" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D40" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E40" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F40" s="6" t="inlineStr">
@@ -1336,17 +1336,17 @@
       <c r="A41" s="5" t="inlineStr"/>
       <c r="B41" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C41" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>192</t>
         </is>
       </c>
       <c r="D41" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>192</t>
         </is>
       </c>
       <c r="E41" s="5" t="inlineStr">
@@ -1364,17 +1364,17 @@
       <c r="A42" s="5" t="inlineStr"/>
       <c r="B42" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C42" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1444</t>
         </is>
       </c>
       <c r="D42" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>1444</t>
         </is>
       </c>
       <c r="E42" s="5" t="inlineStr">
@@ -1392,17 +1392,17 @@
       <c r="A43" s="5" t="inlineStr"/>
       <c r="B43" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C43" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>192</t>
         </is>
       </c>
       <c r="D43" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>192</t>
         </is>
       </c>
       <c r="E43" s="5" t="inlineStr">
@@ -1419,7 +1419,7 @@
     <row r="45">
       <c r="A45" s="4" t="inlineStr">
         <is>
-          <t>UTILES_JARDIN</t>
+          <t>TIERRA_ARIDOS</t>
         </is>
       </c>
     </row>
@@ -1427,22 +1427,22 @@
       <c r="A46" s="5" t="inlineStr"/>
       <c r="B46" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C46" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D46" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E46" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F46" s="6" t="inlineStr">
@@ -1455,22 +1455,22 @@
       <c r="A47" s="5" t="inlineStr"/>
       <c r="B47" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C47" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D47" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E47" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F47" s="6" t="inlineStr">
@@ -1483,22 +1483,22 @@
       <c r="A48" s="5" t="inlineStr"/>
       <c r="B48" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C48" s="5" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D48" s="5" t="inlineStr">
         <is>
-          <t>649</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E48" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F48" s="6" t="inlineStr">
@@ -1511,17 +1511,17 @@
       <c r="A49" s="5" t="inlineStr"/>
       <c r="B49" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C49" s="5" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D49" s="5" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>22</t>
         </is>
       </c>
       <c r="E49" s="5" t="inlineStr">
@@ -1539,17 +1539,17 @@
       <c r="A50" s="5" t="inlineStr"/>
       <c r="B50" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C50" s="5" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="D50" s="5" t="inlineStr">
         <is>
-          <t>35</t>
+          <t>1998</t>
         </is>
       </c>
       <c r="E50" s="5" t="inlineStr">
@@ -1567,17 +1567,17 @@
       <c r="A51" s="5" t="inlineStr"/>
       <c r="B51" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C51" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22</t>
         </is>
       </c>
       <c r="D51" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>22</t>
         </is>
       </c>
       <c r="E51" s="5" t="inlineStr">
@@ -1594,7 +1594,7 @@
     <row r="53">
       <c r="A53" s="4" t="inlineStr">
         <is>
-          <t>INTERIOR</t>
+          <t>MAF</t>
         </is>
       </c>
     </row>
@@ -1602,22 +1602,22 @@
       <c r="A54" s="5" t="inlineStr"/>
       <c r="B54" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C54" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D54" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E54" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F54" s="6" t="inlineStr">
@@ -1630,22 +1630,22 @@
       <c r="A55" s="5" t="inlineStr"/>
       <c r="B55" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C55" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D55" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E55" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F55" s="6" t="inlineStr">
@@ -1658,22 +1658,22 @@
       <c r="A56" s="5" t="inlineStr"/>
       <c r="B56" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C56" s="5" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D56" s="5" t="inlineStr">
         <is>
-          <t>134</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E56" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F56" s="6" t="inlineStr">
@@ -1686,17 +1686,17 @@
       <c r="A57" s="5" t="inlineStr"/>
       <c r="B57" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C57" s="5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D57" s="5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E57" s="5" t="inlineStr">
@@ -1714,17 +1714,17 @@
       <c r="A58" s="5" t="inlineStr"/>
       <c r="B58" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C58" s="5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>148</t>
         </is>
       </c>
       <c r="D58" s="5" t="inlineStr">
         <is>
-          <t>9</t>
+          <t>148</t>
         </is>
       </c>
       <c r="E58" s="5" t="inlineStr">
@@ -1742,17 +1742,17 @@
       <c r="A59" s="5" t="inlineStr"/>
       <c r="B59" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C59" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
         </is>
       </c>
       <c r="D59" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>10</t>
         </is>
       </c>
       <c r="E59" s="5" t="inlineStr">
@@ -1769,7 +1769,7 @@
     <row r="61">
       <c r="A61" s="4" t="inlineStr">
         <is>
-          <t>MAF</t>
+          <t>FITOS</t>
         </is>
       </c>
     </row>
@@ -1777,22 +1777,22 @@
       <c r="A62" s="5" t="inlineStr"/>
       <c r="B62" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C62" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="D62" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="E62" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F62" s="6" t="inlineStr">
@@ -1805,22 +1805,22 @@
       <c r="A63" s="5" t="inlineStr"/>
       <c r="B63" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C63" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D63" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E63" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F63" s="6" t="inlineStr">
@@ -1833,22 +1833,22 @@
       <c r="A64" s="5" t="inlineStr"/>
       <c r="B64" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C64" s="5" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D64" s="5" t="inlineStr">
         <is>
-          <t>148</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E64" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F64" s="6" t="inlineStr">
@@ -1861,17 +1861,17 @@
       <c r="A65" s="5" t="inlineStr"/>
       <c r="B65" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C65" s="5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D65" s="5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E65" s="5" t="inlineStr">
@@ -1889,17 +1889,17 @@
       <c r="A66" s="5" t="inlineStr"/>
       <c r="B66" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C66" s="5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D66" s="5" t="inlineStr">
         <is>
-          <t>10</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E66" s="5" t="inlineStr">
@@ -1917,7 +1917,7 @@
       <c r="A67" s="5" t="inlineStr"/>
       <c r="B67" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C67" s="5" t="inlineStr">
@@ -1944,7 +1944,7 @@
     <row r="69">
       <c r="A69" s="4" t="inlineStr">
         <is>
-          <t>DECO_EXTERIOR</t>
+          <t>MASCOTAS_VIVO</t>
         </is>
       </c>
     </row>
@@ -1952,22 +1952,22 @@
       <c r="A70" s="5" t="inlineStr"/>
       <c r="B70" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C70" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="D70" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>0.0%</t>
         </is>
       </c>
       <c r="E70" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F70" s="6" t="inlineStr">
@@ -1980,22 +1980,22 @@
       <c r="A71" s="5" t="inlineStr"/>
       <c r="B71" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C71" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D71" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E71" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F71" s="6" t="inlineStr">
@@ -2008,27 +2008,27 @@
       <c r="A72" s="5" t="inlineStr"/>
       <c r="B72" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C72" s="5" t="inlineStr">
         <is>
-          <t>1753</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D72" s="5" t="inlineStr">
         <is>
-          <t>1542</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E72" s="5" t="inlineStr">
         <is>
-          <t>-211</t>
-        </is>
-      </c>
-      <c r="F72" s="8" t="inlineStr">
-        <is>
-          <t>↓</t>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="F72" s="6" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -2036,27 +2036,27 @@
       <c r="A73" s="5" t="inlineStr"/>
       <c r="B73" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C73" s="5" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D73" s="5" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E73" s="5" t="inlineStr">
         <is>
-          <t>+10</t>
-        </is>
-      </c>
-      <c r="F73" s="7" t="inlineStr">
-        <is>
-          <t>↑</t>
+          <t>+0</t>
+        </is>
+      </c>
+      <c r="F73" s="6" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -2064,27 +2064,27 @@
       <c r="A74" s="5" t="inlineStr"/>
       <c r="B74" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C74" s="5" t="inlineStr">
         <is>
-          <t>52</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D74" s="5" t="inlineStr">
         <is>
-          <t>62</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E74" s="5" t="inlineStr">
         <is>
-          <t>+10</t>
-        </is>
-      </c>
-      <c r="F74" s="7" t="inlineStr">
-        <is>
-          <t>↑</t>
+          <t>+0</t>
+        </is>
+      </c>
+      <c r="F74" s="6" t="inlineStr">
+        <is>
+          <t>=</t>
         </is>
       </c>
     </row>
@@ -2092,7 +2092,7 @@
       <c r="A75" s="5" t="inlineStr"/>
       <c r="B75" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C75" s="5" t="inlineStr">
@@ -2119,7 +2119,7 @@
     <row r="77">
       <c r="A77" s="4" t="inlineStr">
         <is>
-          <t>MASCOTAS_MANUFACTURADO</t>
+          <t>INTERIOR</t>
         </is>
       </c>
     </row>
@@ -2127,22 +2127,22 @@
       <c r="A78" s="5" t="inlineStr"/>
       <c r="B78" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C78" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D78" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E78" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F78" s="6" t="inlineStr">
@@ -2155,22 +2155,22 @@
       <c r="A79" s="5" t="inlineStr"/>
       <c r="B79" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C79" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D79" s="5" t="inlineStr">
         <is>
-          <t>100.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E79" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F79" s="6" t="inlineStr">
@@ -2183,22 +2183,22 @@
       <c r="A80" s="5" t="inlineStr"/>
       <c r="B80" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C80" s="5" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D80" s="5" t="inlineStr">
         <is>
-          <t>1444</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E80" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F80" s="6" t="inlineStr">
@@ -2211,17 +2211,17 @@
       <c r="A81" s="5" t="inlineStr"/>
       <c r="B81" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C81" s="5" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D81" s="5" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E81" s="5" t="inlineStr">
@@ -2239,17 +2239,17 @@
       <c r="A82" s="5" t="inlineStr"/>
       <c r="B82" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C82" s="5" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>134</t>
         </is>
       </c>
       <c r="D82" s="5" t="inlineStr">
         <is>
-          <t>192</t>
+          <t>134</t>
         </is>
       </c>
       <c r="E82" s="5" t="inlineStr">
@@ -2267,17 +2267,17 @@
       <c r="A83" s="5" t="inlineStr"/>
       <c r="B83" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C83" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="D83" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>9</t>
         </is>
       </c>
       <c r="E83" s="5" t="inlineStr">
@@ -2294,7 +2294,7 @@
     <row r="85">
       <c r="A85" s="4" t="inlineStr">
         <is>
-          <t>FITOS</t>
+          <t>UTILES_JARDIN</t>
         </is>
       </c>
     </row>
@@ -2302,22 +2302,22 @@
       <c r="A86" s="5" t="inlineStr"/>
       <c r="B86" s="5" t="inlineStr">
         <is>
-          <t>Métrica</t>
+          <t>Porcentaje sin eliminar (%)</t>
         </is>
       </c>
       <c r="C86" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="D86" s="5" t="inlineStr">
         <is>
-          <t>Valor</t>
+          <t>100.0%</t>
         </is>
       </c>
       <c r="E86" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>+0.0%</t>
         </is>
       </c>
       <c r="F86" s="6" t="inlineStr">
@@ -2330,22 +2330,22 @@
       <c r="A87" s="5" t="inlineStr"/>
       <c r="B87" s="5" t="inlineStr">
         <is>
-          <t>Porcentaje sin eliminar (%)</t>
+          <t>Artículos ya eliminados del stock</t>
         </is>
       </c>
       <c r="C87" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="D87" s="5" t="inlineStr">
         <is>
-          <t>0.0%</t>
+          <t>0</t>
         </is>
       </c>
       <c r="E87" s="5" t="inlineStr">
         <is>
-          <t>+0.0%</t>
+          <t>+0</t>
         </is>
       </c>
       <c r="F87" s="6" t="inlineStr">
@@ -2358,22 +2358,22 @@
       <c r="A88" s="5" t="inlineStr"/>
       <c r="B88" s="5" t="inlineStr">
         <is>
-          <t>Unidades totales en stock</t>
+          <t>Métrica</t>
         </is>
       </c>
       <c r="C88" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="D88" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>Valor</t>
         </is>
       </c>
       <c r="E88" s="5" t="inlineStr">
         <is>
-          <t>+0</t>
+          <t>0</t>
         </is>
       </c>
       <c r="F88" s="6" t="inlineStr">
@@ -2386,17 +2386,17 @@
       <c r="A89" s="5" t="inlineStr"/>
       <c r="B89" s="5" t="inlineStr">
         <is>
-          <t>Total artículos C+D identificados</t>
+          <t>Artículos todavía en stock</t>
         </is>
       </c>
       <c r="C89" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D89" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E89" s="5" t="inlineStr">
@@ -2414,17 +2414,17 @@
       <c r="A90" s="5" t="inlineStr"/>
       <c r="B90" s="5" t="inlineStr">
         <is>
-          <t>Artículos todavía en stock</t>
+          <t>Unidades totales en stock</t>
         </is>
       </c>
       <c r="C90" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>649</t>
         </is>
       </c>
       <c r="D90" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>649</t>
         </is>
       </c>
       <c r="E90" s="5" t="inlineStr">
@@ -2442,17 +2442,17 @@
       <c r="A91" s="5" t="inlineStr"/>
       <c r="B91" s="5" t="inlineStr">
         <is>
-          <t>Artículos ya eliminados del stock</t>
+          <t>Total artículos C+D identificados</t>
         </is>
       </c>
       <c r="C91" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35</t>
         </is>
       </c>
       <c r="D91" s="5" t="inlineStr">
         <is>
-          <t>0</t>
+          <t>35</t>
         </is>
       </c>
       <c r="E91" s="5" t="inlineStr">

</xml_diff>